<commit_message>
Optimized julia ODE solving with tmap
</commit_message>
<xml_diff>
--- a/Data/Human Data Summary.xlsx
+++ b/Data/Human Data Summary.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveutk-my.sharepoint.com/personal/jweave49_uthsc_edu/Documents/VPC/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Documents\GitHub\VPC\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="882" documentId="13_ncr:1_{382891BB-CC8A-4A49-9DFC-5B904B79D3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B64BBEE0-8DB9-4A7F-BC03-50E7E58D817F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA9743C-76A6-4124-A48B-5E728F762A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{898542A7-1ACD-6F4C-AB87-2AD8DF6B2639}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{898542A7-1ACD-6F4C-AB87-2AD8DF6B2639}"/>
   </bookViews>
   <sheets>
     <sheet name="Influenza Infection" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Influenza Infection'!$C$1:$AH$1</definedName>
@@ -60,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="272">
   <si>
     <t>Details</t>
   </si>
@@ -1356,9 +1354,9 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD1" sqref="A1:AD1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3283,1122 +3281,4 @@
   <pageSetup scale="35" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384395F9-C7DD-4BA2-A147-80688BC6CA00}">
-  <dimension ref="A1:H40"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:H40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="30.625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7662AA33-AADA-465D-B0B7-E69C4294EF20}">
-  <dimension ref="A1:H56"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:H35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.25" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="2" customWidth="1"/>
-    <col min="6" max="8" width="9.5" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>